<commit_message>
Manual pub b/c CI/CD down due to pubpack issue.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-PublicHealthMeasure.xlsx
+++ b/docs/StructureDefinition-PublicHealthMeasure.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$156</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5020" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5407" uniqueCount="566">
   <si>
     <t>Path</t>
   </si>
@@ -1359,9 +1359,6 @@
     <t>Measure.group.population.code.coding</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coding
 </t>
   </si>
@@ -1513,7 +1510,7 @@
     <t>Measure.group.stratifier</t>
   </si>
   <si>
-    <t>Stratifier criteria for the measure</t>
+    <t>A group may have none, some or many strata</t>
   </si>
   <si>
     <t>The stratifier criteria for the measure report, specified as either the name of a valid CQL expression defined within a referenced library or a valid FHIR Resource Path.</t>
@@ -1531,16 +1528,136 @@
     <t>Measure.group.stratifier.code</t>
   </si>
   <si>
-    <t>Meaning of the stratifier</t>
+    <t>Describes the purpose of this stratifier</t>
   </si>
   <si>
     <t>Indicates a meaning for the stratifier. This can be as simple as a unique identifier, or it can establish meaning in a broader context by drawing from a terminology, allowing stratifiers to be correlated across measures.</t>
   </si>
   <si>
+    <t>Measure.group.stratifier.code.id</t>
+  </si>
+  <si>
+    <t>Measure.group.stratifier.code.extension</t>
+  </si>
+  <si>
+    <t>Measure.group.stratifier.code.coding</t>
+  </si>
+  <si>
+    <t>Uniquely identifies the strata</t>
+  </si>
+  <si>
+    <t>Measure.group.stratifier.code.coding.id</t>
+  </si>
+  <si>
+    <t>Measure.group.stratifier.code.coding.extension</t>
+  </si>
+  <si>
+    <t>Measure.group.stratifier.code.coding.system</t>
+  </si>
+  <si>
+    <t>Identity of the terminology system</t>
+  </si>
+  <si>
+    <t>The identification of the code system that defines the meaning of the symbol in the code.</t>
+  </si>
+  <si>
+    <t>The URI may be an OID (urn:oid:...) or a UUID (urn:uuid:...).  OIDs and UUIDs SHALL be references to the HL7 OID registry. Otherwise, the URI should come from HL7's list of FHIR defined special URIs or it should reference to some definition that establishes the system clearly and unambiguously.</t>
+  </si>
+  <si>
+    <t>Need to be unambiguous about the source of the definition of the symbol.</t>
+  </si>
+  <si>
+    <t>Coding.system</t>
+  </si>
+  <si>
+    <t>./codeSystem</t>
+  </si>
+  <si>
+    <t>Measure.group.stratifier.code.coding.version</t>
+  </si>
+  <si>
+    <t>Version of the system - if relevant</t>
+  </si>
+  <si>
+    <t>The version of the code system which was used when choosing this code. Note that a well-maintained code system does not need the version reported, because the meaning of codes is consistent across versions. However this cannot consistently be assured, and when the meaning is not guaranteed to be consistent, the version SHOULD be exchanged.</t>
+  </si>
+  <si>
+    <t>Where the terminology does not clearly define what string should be used to identify code system versions, the recommendation is to use the date (expressed in FHIR date format) on which that version was officially published as the version date.</t>
+  </si>
+  <si>
+    <t>Coding.version</t>
+  </si>
+  <si>
+    <t>./codeSystemVersion</t>
+  </si>
+  <si>
+    <t>Measure.group.stratifier.code.coding.code</t>
+  </si>
+  <si>
+    <t>Symbol in syntax defined by the system</t>
+  </si>
+  <si>
+    <t>A symbol in syntax defined by the system. The symbol may be a predefined code or an expression in a syntax defined by the coding system (e.g. post-coordination).</t>
+  </si>
+  <si>
+    <t>Need to refer to a particular code in the system.</t>
+  </si>
+  <si>
+    <t>Coding.code</t>
+  </si>
+  <si>
+    <t>./code</t>
+  </si>
+  <si>
+    <t>Measure.group.stratifier.code.coding.display</t>
+  </si>
+  <si>
+    <t>Provides a human readable name for the strata</t>
+  </si>
+  <si>
+    <t>A representation of the meaning of the code in the system, following the rules of the system.</t>
+  </si>
+  <si>
+    <t>Need to be able to carry a human-readable meaning of the code for readers that do not know  the system.</t>
+  </si>
+  <si>
+    <t>Coding.display</t>
+  </si>
+  <si>
+    <t>CV.displayName</t>
+  </si>
+  <si>
+    <t>Measure.group.stratifier.code.coding.userSelected</t>
+  </si>
+  <si>
+    <t>If this coding was chosen directly by the user</t>
+  </si>
+  <si>
+    <t>Indicates that this coding was chosen by a user directly - e.g. off a pick list of available items (codes or displays).</t>
+  </si>
+  <si>
+    <t>Amongst a set of alternatives, a directly chosen code is the most appropriate starting point for new translations. There is some ambiguity about what exactly 'directly chosen' implies, and trading partner agreement may be needed to clarify the use of this element and its consequences more completely.</t>
+  </si>
+  <si>
+    <t>This has been identified as a clinical safety criterium - that this exact system/code pair was chosen explicitly, rather than inferred by the system based on some rules or language processing.</t>
+  </si>
+  <si>
+    <t>Coding.userSelected</t>
+  </si>
+  <si>
+    <t>CD.codingRationale</t>
+  </si>
+  <si>
+    <t>Measure.group.stratifier.code.text</t>
+  </si>
+  <si>
+    <t>Describes the function of the stratifier.</t>
+  </si>
+  <si>
     <t>Measure.group.stratifier.description</t>
   </si>
   <si>
-    <t>The human readable description of this stratifier</t>
+    <t>Describes the overall function of the strata.</t>
   </si>
   <si>
     <t>The human readable description of this stratifier criteria.</t>
@@ -1562,7 +1679,7 @@
     <t>Measure.group.stratifier.component</t>
   </si>
   <si>
-    <t>Stratifier criteria component for the measure</t>
+    <t>A stratifier must have at least one stratum</t>
   </si>
   <si>
     <t>A component of the stratifier criteria for the measure report, specified as either the name of a valid CQL expression defined within a referenced library or a valid FHIR Resource Path.</t>
@@ -1592,7 +1709,7 @@
     <t>Measure.group.stratifier.component.description</t>
   </si>
   <si>
-    <t>The human readable description of this stratifier component</t>
+    <t>Describes the purpose of this stratum</t>
   </si>
   <si>
     <t>The human readable description of this stratifier criteria component.</t>
@@ -1816,7 +1933,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM145"/>
+  <dimension ref="A1:AM156"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -14228,7 +14345,7 @@
       </c>
       <c r="D113" s="2"/>
       <c r="E113" t="s" s="2">
-        <v>425</v>
+        <v>48</v>
       </c>
       <c r="F113" t="s" s="2">
         <v>42</v>
@@ -14243,19 +14360,19 @@
         <v>49</v>
       </c>
       <c r="J113" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="K113" t="s" s="2">
         <v>426</v>
       </c>
-      <c r="K113" t="s" s="2">
+      <c r="L113" t="s" s="2">
         <v>427</v>
       </c>
-      <c r="L113" t="s" s="2">
+      <c r="M113" t="s" s="2">
         <v>428</v>
       </c>
-      <c r="M113" t="s" s="2">
+      <c r="N113" t="s" s="2">
         <v>429</v>
-      </c>
-      <c r="N113" t="s" s="2">
-        <v>430</v>
       </c>
       <c r="O113" t="s" s="2">
         <v>40</v>
@@ -14304,7 +14421,7 @@
         <v>40</v>
       </c>
       <c r="AE113" t="s" s="2">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="AF113" t="s" s="2">
         <v>41</v>
@@ -14328,12 +14445,12 @@
         <v>40</v>
       </c>
       <c r="AM113" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" t="s" s="2">
@@ -14359,16 +14476,16 @@
         <v>50</v>
       </c>
       <c r="K114" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="L114" t="s" s="2">
         <v>434</v>
       </c>
-      <c r="L114" t="s" s="2">
+      <c r="M114" t="s" s="2">
         <v>435</v>
       </c>
-      <c r="M114" t="s" s="2">
+      <c r="N114" t="s" s="2">
         <v>436</v>
-      </c>
-      <c r="N114" t="s" s="2">
-        <v>437</v>
       </c>
       <c r="O114" t="s" s="2">
         <v>40</v>
@@ -14417,7 +14534,7 @@
         <v>40</v>
       </c>
       <c r="AE114" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AF114" t="s" s="2">
         <v>41</v>
@@ -14441,12 +14558,12 @@
         <v>40</v>
       </c>
       <c r="AM114" t="s" s="2">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" t="s" s="2">
@@ -14472,10 +14589,10 @@
         <v>50</v>
       </c>
       <c r="K115" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="L115" t="s" s="2">
         <v>441</v>
-      </c>
-      <c r="L115" t="s" s="2">
-        <v>442</v>
       </c>
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
@@ -14526,7 +14643,7 @@
         <v>40</v>
       </c>
       <c r="AE115" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AF115" t="s" s="2">
         <v>41</v>
@@ -14555,7 +14672,7 @@
     </row>
     <row r="116" hidden="true">
       <c r="A116" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" t="s" s="2">
@@ -14578,16 +14695,16 @@
         <v>40</v>
       </c>
       <c r="J116" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="K116" t="s" s="2">
         <v>444</v>
       </c>
-      <c r="K116" t="s" s="2">
+      <c r="L116" t="s" s="2">
         <v>445</v>
       </c>
-      <c r="L116" t="s" s="2">
+      <c r="M116" t="s" s="2">
         <v>446</v>
-      </c>
-      <c r="M116" t="s" s="2">
-        <v>447</v>
       </c>
       <c r="N116" s="2"/>
       <c r="O116" t="s" s="2">
@@ -14637,7 +14754,7 @@
         <v>40</v>
       </c>
       <c r="AE116" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AF116" t="s" s="2">
         <v>48</v>
@@ -14649,7 +14766,7 @@
         <v>354</v>
       </c>
       <c r="AI116" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="AJ116" t="s" s="2">
         <v>40</v>
@@ -14666,7 +14783,7 @@
     </row>
     <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" t="s" s="2">
@@ -14775,7 +14892,7 @@
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" t="s" s="2">
@@ -14886,7 +15003,7 @@
     </row>
     <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" t="s" s="2">
@@ -14912,10 +15029,10 @@
         <v>50</v>
       </c>
       <c r="K119" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="L119" t="s" s="2">
         <v>452</v>
-      </c>
-      <c r="L119" t="s" s="2">
-        <v>453</v>
       </c>
       <c r="M119" s="2"/>
       <c r="N119" s="2"/>
@@ -14966,7 +15083,7 @@
         <v>40</v>
       </c>
       <c r="AE119" t="s" s="2">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="AF119" t="s" s="2">
         <v>41</v>
@@ -14995,7 +15112,7 @@
     </row>
     <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" t="s" s="2">
@@ -15018,13 +15135,13 @@
         <v>49</v>
       </c>
       <c r="J120" t="s" s="2">
+        <v>455</v>
+      </c>
+      <c r="K120" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="L120" t="s" s="2">
         <v>456</v>
-      </c>
-      <c r="K120" t="s" s="2">
-        <v>445</v>
-      </c>
-      <c r="L120" t="s" s="2">
-        <v>457</v>
       </c>
       <c r="M120" s="2"/>
       <c r="N120" s="2"/>
@@ -15075,7 +15192,7 @@
         <v>40</v>
       </c>
       <c r="AE120" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AF120" t="s" s="2">
         <v>41</v>
@@ -15104,7 +15221,7 @@
     </row>
     <row r="121" hidden="true">
       <c r="A121" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B121" s="2"/>
       <c r="C121" t="s" s="2">
@@ -15130,10 +15247,10 @@
         <v>68</v>
       </c>
       <c r="K121" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="L121" t="s" s="2">
         <v>460</v>
-      </c>
-      <c r="L121" t="s" s="2">
-        <v>461</v>
       </c>
       <c r="M121" s="2"/>
       <c r="N121" s="2"/>
@@ -15163,28 +15280,28 @@
         <v>162</v>
       </c>
       <c r="X121" t="s" s="2">
+        <v>461</v>
+      </c>
+      <c r="Y121" t="s" s="2">
         <v>462</v>
       </c>
-      <c r="Y121" t="s" s="2">
+      <c r="Z121" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA121" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB121" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC121" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD121" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE121" t="s" s="2">
         <v>463</v>
-      </c>
-      <c r="Z121" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA121" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB121" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC121" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD121" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE121" t="s" s="2">
-        <v>464</v>
       </c>
       <c r="AF121" t="s" s="2">
         <v>48</v>
@@ -15213,7 +15330,7 @@
     </row>
     <row r="122" hidden="true">
       <c r="A122" t="s" s="2">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" t="s" s="2">
@@ -15239,10 +15356,10 @@
         <v>50</v>
       </c>
       <c r="K122" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="L122" t="s" s="2">
         <v>466</v>
-      </c>
-      <c r="L122" t="s" s="2">
-        <v>467</v>
       </c>
       <c r="M122" s="2"/>
       <c r="N122" s="2"/>
@@ -15293,7 +15410,7 @@
         <v>40</v>
       </c>
       <c r="AE122" t="s" s="2">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AF122" t="s" s="2">
         <v>41</v>
@@ -15322,7 +15439,7 @@
     </row>
     <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" t="s" s="2">
@@ -15348,13 +15465,13 @@
         <v>62</v>
       </c>
       <c r="K123" t="s" s="2">
+        <v>469</v>
+      </c>
+      <c r="L123" t="s" s="2">
         <v>470</v>
       </c>
-      <c r="L123" t="s" s="2">
+      <c r="M123" t="s" s="2">
         <v>471</v>
-      </c>
-      <c r="M123" t="s" s="2">
-        <v>472</v>
       </c>
       <c r="N123" s="2"/>
       <c r="O123" t="s" s="2">
@@ -15404,7 +15521,7 @@
         <v>40</v>
       </c>
       <c r="AE123" t="s" s="2">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="AF123" t="s" s="2">
         <v>41</v>
@@ -15433,7 +15550,7 @@
     </row>
     <row r="124" hidden="true">
       <c r="A124" t="s" s="2">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" t="s" s="2">
@@ -15459,10 +15576,10 @@
         <v>343</v>
       </c>
       <c r="K124" t="s" s="2">
+        <v>474</v>
+      </c>
+      <c r="L124" t="s" s="2">
         <v>475</v>
-      </c>
-      <c r="L124" t="s" s="2">
-        <v>476</v>
       </c>
       <c r="M124" s="2"/>
       <c r="N124" s="2"/>
@@ -15513,7 +15630,7 @@
         <v>40</v>
       </c>
       <c r="AE124" t="s" s="2">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AF124" t="s" s="2">
         <v>41</v>
@@ -15542,7 +15659,7 @@
     </row>
     <row r="125" hidden="true">
       <c r="A125" t="s" s="2">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" t="s" s="2">
@@ -15651,7 +15768,7 @@
     </row>
     <row r="126" hidden="true">
       <c r="A126" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" t="s" s="2">
@@ -15762,7 +15879,7 @@
     </row>
     <row r="127" hidden="true">
       <c r="A127" t="s" s="2">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" t="s" s="2">
@@ -15875,7 +15992,7 @@
     </row>
     <row r="128" hidden="true">
       <c r="A128" t="s" s="2">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" t="s" s="2">
@@ -15883,7 +16000,7 @@
       </c>
       <c r="D128" s="2"/>
       <c r="E128" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F128" t="s" s="2">
         <v>48</v>
@@ -15901,10 +16018,10 @@
         <v>200</v>
       </c>
       <c r="K128" t="s" s="2">
+        <v>480</v>
+      </c>
+      <c r="L128" t="s" s="2">
         <v>481</v>
-      </c>
-      <c r="L128" t="s" s="2">
-        <v>482</v>
       </c>
       <c r="M128" s="2"/>
       <c r="N128" s="2"/>
@@ -15955,7 +16072,7 @@
         <v>40</v>
       </c>
       <c r="AE128" t="s" s="2">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AF128" t="s" s="2">
         <v>41</v>
@@ -15984,7 +16101,7 @@
     </row>
     <row r="129" hidden="true">
       <c r="A129" t="s" s="2">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" t="s" s="2">
@@ -16010,10 +16127,10 @@
         <v>50</v>
       </c>
       <c r="K129" t="s" s="2">
-        <v>484</v>
+        <v>253</v>
       </c>
       <c r="L129" t="s" s="2">
-        <v>485</v>
+        <v>254</v>
       </c>
       <c r="M129" s="2"/>
       <c r="N129" s="2"/>
@@ -16064,7 +16181,7 @@
         <v>40</v>
       </c>
       <c r="AE129" t="s" s="2">
-        <v>483</v>
+        <v>255</v>
       </c>
       <c r="AF129" t="s" s="2">
         <v>41</v>
@@ -16076,7 +16193,7 @@
         <v>40</v>
       </c>
       <c r="AI129" t="s" s="2">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="AJ129" t="s" s="2">
         <v>40</v>
@@ -16088,23 +16205,23 @@
         <v>40</v>
       </c>
       <c r="AM129" t="s" s="2">
-        <v>40</v>
+        <v>256</v>
       </c>
     </row>
     <row r="130" hidden="true">
       <c r="A130" t="s" s="2">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" t="s" s="2">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="D130" s="2"/>
       <c r="E130" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F130" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G130" t="s" s="2">
         <v>40</v>
@@ -16116,15 +16233,17 @@
         <v>40</v>
       </c>
       <c r="J130" t="s" s="2">
-        <v>487</v>
+        <v>94</v>
       </c>
       <c r="K130" t="s" s="2">
-        <v>488</v>
+        <v>95</v>
       </c>
       <c r="L130" t="s" s="2">
-        <v>489</v>
-      </c>
-      <c r="M130" s="2"/>
+        <v>258</v>
+      </c>
+      <c r="M130" t="s" s="2">
+        <v>97</v>
+      </c>
       <c r="N130" s="2"/>
       <c r="O130" t="s" s="2">
         <v>40</v>
@@ -16161,31 +16280,31 @@
         <v>40</v>
       </c>
       <c r="AA130" t="s" s="2">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="AB130" t="s" s="2">
-        <v>40</v>
+        <v>260</v>
       </c>
       <c r="AC130" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD130" t="s" s="2">
-        <v>40</v>
+        <v>261</v>
       </c>
       <c r="AE130" t="s" s="2">
-        <v>486</v>
+        <v>262</v>
       </c>
       <c r="AF130" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG130" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="AH130" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI130" t="s" s="2">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="AJ130" t="s" s="2">
         <v>40</v>
@@ -16197,12 +16316,12 @@
         <v>40</v>
       </c>
       <c r="AM130" t="s" s="2">
-        <v>40</v>
+        <v>256</v>
       </c>
     </row>
     <row r="131" hidden="true">
       <c r="A131" t="s" s="2">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="B131" s="2"/>
       <c r="C131" t="s" s="2">
@@ -16210,7 +16329,7 @@
       </c>
       <c r="D131" s="2"/>
       <c r="E131" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F131" t="s" s="2">
         <v>42</v>
@@ -16222,21 +16341,23 @@
         <v>40</v>
       </c>
       <c r="I131" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J131" t="s" s="2">
-        <v>343</v>
+        <v>425</v>
       </c>
       <c r="K131" t="s" s="2">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="L131" t="s" s="2">
-        <v>492</v>
+        <v>427</v>
       </c>
       <c r="M131" t="s" s="2">
-        <v>493</v>
-      </c>
-      <c r="N131" s="2"/>
+        <v>428</v>
+      </c>
+      <c r="N131" t="s" s="2">
+        <v>429</v>
+      </c>
       <c r="O131" t="s" s="2">
         <v>40</v>
       </c>
@@ -16284,7 +16405,7 @@
         <v>40</v>
       </c>
       <c r="AE131" t="s" s="2">
-        <v>490</v>
+        <v>430</v>
       </c>
       <c r="AF131" t="s" s="2">
         <v>41</v>
@@ -16308,12 +16429,12 @@
         <v>40</v>
       </c>
       <c r="AM131" t="s" s="2">
-        <v>40</v>
+        <v>431</v>
       </c>
     </row>
     <row r="132" hidden="true">
       <c r="A132" t="s" s="2">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B132" s="2"/>
       <c r="C132" t="s" s="2">
@@ -16422,7 +16543,7 @@
     </row>
     <row r="133" hidden="true">
       <c r="A133" t="s" s="2">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="B133" s="2"/>
       <c r="C133" t="s" s="2">
@@ -16492,16 +16613,16 @@
         <v>40</v>
       </c>
       <c r="AA133" t="s" s="2">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="AB133" t="s" s="2">
-        <v>40</v>
+        <v>260</v>
       </c>
       <c r="AC133" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD133" t="s" s="2">
-        <v>40</v>
+        <v>261</v>
       </c>
       <c r="AE133" t="s" s="2">
         <v>262</v>
@@ -16533,42 +16654,42 @@
     </row>
     <row r="134" hidden="true">
       <c r="A134" t="s" s="2">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" t="s" s="2">
-        <v>399</v>
+        <v>40</v>
       </c>
       <c r="D134" s="2"/>
       <c r="E134" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F134" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G134" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H134" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="I134" t="s" s="2">
         <v>49</v>
       </c>
       <c r="J134" t="s" s="2">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="K134" t="s" s="2">
-        <v>400</v>
+        <v>489</v>
       </c>
       <c r="L134" t="s" s="2">
-        <v>401</v>
+        <v>490</v>
       </c>
       <c r="M134" t="s" s="2">
-        <v>97</v>
+        <v>491</v>
       </c>
       <c r="N134" t="s" s="2">
-        <v>103</v>
+        <v>492</v>
       </c>
       <c r="O134" t="s" s="2">
         <v>40</v>
@@ -16617,19 +16738,19 @@
         <v>40</v>
       </c>
       <c r="AE134" t="s" s="2">
-        <v>402</v>
+        <v>493</v>
       </c>
       <c r="AF134" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG134" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="AH134" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI134" t="s" s="2">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="AJ134" t="s" s="2">
         <v>40</v>
@@ -16641,12 +16762,12 @@
         <v>40</v>
       </c>
       <c r="AM134" t="s" s="2">
-        <v>91</v>
+        <v>494</v>
       </c>
     </row>
     <row r="135" hidden="true">
       <c r="A135" t="s" s="2">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" t="s" s="2">
@@ -16666,18 +16787,20 @@
         <v>40</v>
       </c>
       <c r="I135" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J135" t="s" s="2">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="K135" t="s" s="2">
+        <v>496</v>
+      </c>
+      <c r="L135" t="s" s="2">
+        <v>497</v>
+      </c>
+      <c r="M135" t="s" s="2">
         <v>498</v>
       </c>
-      <c r="L135" t="s" s="2">
-        <v>499</v>
-      </c>
-      <c r="M135" s="2"/>
       <c r="N135" s="2"/>
       <c r="O135" t="s" s="2">
         <v>40</v>
@@ -16726,7 +16849,7 @@
         <v>40</v>
       </c>
       <c r="AE135" t="s" s="2">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="AF135" t="s" s="2">
         <v>41</v>
@@ -16750,12 +16873,12 @@
         <v>40</v>
       </c>
       <c r="AM135" t="s" s="2">
-        <v>40</v>
+        <v>500</v>
       </c>
     </row>
     <row r="136" hidden="true">
       <c r="A136" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" t="s" s="2">
@@ -16775,19 +16898,21 @@
         <v>40</v>
       </c>
       <c r="I136" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J136" t="s" s="2">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="K136" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="L136" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="M136" s="2"/>
-      <c r="N136" s="2"/>
+      <c r="N136" t="s" s="2">
+        <v>504</v>
+      </c>
       <c r="O136" t="s" s="2">
         <v>40</v>
       </c>
@@ -16835,7 +16960,7 @@
         <v>40</v>
       </c>
       <c r="AE136" t="s" s="2">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="AF136" t="s" s="2">
         <v>41</v>
@@ -16859,12 +16984,12 @@
         <v>40</v>
       </c>
       <c r="AM136" t="s" s="2">
-        <v>40</v>
+        <v>506</v>
       </c>
     </row>
     <row r="137" hidden="true">
       <c r="A137" t="s" s="2">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="B137" s="2"/>
       <c r="C137" t="s" s="2">
@@ -16884,19 +17009,21 @@
         <v>40</v>
       </c>
       <c r="I137" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J137" t="s" s="2">
-        <v>487</v>
+        <v>50</v>
       </c>
       <c r="K137" t="s" s="2">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="L137" t="s" s="2">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="M137" s="2"/>
-      <c r="N137" s="2"/>
+      <c r="N137" t="s" s="2">
+        <v>510</v>
+      </c>
       <c r="O137" t="s" s="2">
         <v>40</v>
       </c>
@@ -16944,10 +17071,10 @@
         <v>40</v>
       </c>
       <c r="AE137" t="s" s="2">
-        <v>503</v>
+        <v>511</v>
       </c>
       <c r="AF137" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="AG137" t="s" s="2">
         <v>48</v>
@@ -16968,12 +17095,12 @@
         <v>40</v>
       </c>
       <c r="AM137" t="s" s="2">
-        <v>40</v>
+        <v>512</v>
       </c>
     </row>
     <row r="138" hidden="true">
       <c r="A138" t="s" s="2">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="B138" s="2"/>
       <c r="C138" t="s" s="2">
@@ -16984,7 +17111,7 @@
         <v>41</v>
       </c>
       <c r="F138" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G138" t="s" s="2">
         <v>40</v>
@@ -16993,21 +17120,23 @@
         <v>40</v>
       </c>
       <c r="I138" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J138" t="s" s="2">
-        <v>343</v>
+        <v>149</v>
       </c>
       <c r="K138" t="s" s="2">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="L138" t="s" s="2">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="M138" t="s" s="2">
-        <v>509</v>
-      </c>
-      <c r="N138" s="2"/>
+        <v>516</v>
+      </c>
+      <c r="N138" t="s" s="2">
+        <v>517</v>
+      </c>
       <c r="O138" t="s" s="2">
         <v>40</v>
       </c>
@@ -17055,13 +17184,13 @@
         <v>40</v>
       </c>
       <c r="AE138" t="s" s="2">
-        <v>506</v>
+        <v>518</v>
       </c>
       <c r="AF138" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG138" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="AH138" t="s" s="2">
         <v>40</v>
@@ -17079,12 +17208,12 @@
         <v>40</v>
       </c>
       <c r="AM138" t="s" s="2">
-        <v>40</v>
+        <v>519</v>
       </c>
     </row>
     <row r="139" hidden="true">
       <c r="A139" t="s" s="2">
-        <v>510</v>
+        <v>520</v>
       </c>
       <c r="B139" s="2"/>
       <c r="C139" t="s" s="2">
@@ -17104,19 +17233,23 @@
         <v>40</v>
       </c>
       <c r="I139" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J139" t="s" s="2">
         <v>50</v>
       </c>
       <c r="K139" t="s" s="2">
-        <v>253</v>
+        <v>521</v>
       </c>
       <c r="L139" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="M139" s="2"/>
-      <c r="N139" s="2"/>
+        <v>434</v>
+      </c>
+      <c r="M139" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="N139" t="s" s="2">
+        <v>436</v>
+      </c>
       <c r="O139" t="s" s="2">
         <v>40</v>
       </c>
@@ -17164,7 +17297,7 @@
         <v>40</v>
       </c>
       <c r="AE139" t="s" s="2">
-        <v>255</v>
+        <v>437</v>
       </c>
       <c r="AF139" t="s" s="2">
         <v>41</v>
@@ -17176,7 +17309,7 @@
         <v>40</v>
       </c>
       <c r="AI139" t="s" s="2">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="AJ139" t="s" s="2">
         <v>40</v>
@@ -17188,23 +17321,23 @@
         <v>40</v>
       </c>
       <c r="AM139" t="s" s="2">
-        <v>256</v>
+        <v>438</v>
       </c>
     </row>
     <row r="140" hidden="true">
       <c r="A140" t="s" s="2">
-        <v>511</v>
+        <v>522</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" t="s" s="2">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="D140" s="2"/>
       <c r="E140" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F140" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G140" t="s" s="2">
         <v>40</v>
@@ -17216,17 +17349,15 @@
         <v>40</v>
       </c>
       <c r="J140" t="s" s="2">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="K140" t="s" s="2">
-        <v>95</v>
+        <v>523</v>
       </c>
       <c r="L140" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="M140" t="s" s="2">
-        <v>97</v>
-      </c>
+        <v>524</v>
+      </c>
+      <c r="M140" s="2"/>
       <c r="N140" s="2"/>
       <c r="O140" t="s" s="2">
         <v>40</v>
@@ -17275,19 +17406,19 @@
         <v>40</v>
       </c>
       <c r="AE140" t="s" s="2">
-        <v>262</v>
+        <v>522</v>
       </c>
       <c r="AF140" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG140" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="AH140" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI140" t="s" s="2">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="AJ140" t="s" s="2">
         <v>40</v>
@@ -17299,48 +17430,44 @@
         <v>40</v>
       </c>
       <c r="AM140" t="s" s="2">
-        <v>256</v>
+        <v>40</v>
       </c>
     </row>
     <row r="141" hidden="true">
       <c r="A141" t="s" s="2">
-        <v>512</v>
+        <v>525</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" t="s" s="2">
-        <v>399</v>
+        <v>40</v>
       </c>
       <c r="D141" s="2"/>
       <c r="E141" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F141" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G141" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H141" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="I141" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="J141" t="s" s="2">
-        <v>94</v>
+        <v>526</v>
       </c>
       <c r="K141" t="s" s="2">
-        <v>400</v>
+        <v>527</v>
       </c>
       <c r="L141" t="s" s="2">
-        <v>401</v>
-      </c>
-      <c r="M141" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="N141" t="s" s="2">
-        <v>103</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="M141" s="2"/>
+      <c r="N141" s="2"/>
       <c r="O141" t="s" s="2">
         <v>40</v>
       </c>
@@ -17388,19 +17515,19 @@
         <v>40</v>
       </c>
       <c r="AE141" t="s" s="2">
-        <v>402</v>
+        <v>525</v>
       </c>
       <c r="AF141" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG141" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="AH141" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI141" t="s" s="2">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="AJ141" t="s" s="2">
         <v>40</v>
@@ -17412,12 +17539,12 @@
         <v>40</v>
       </c>
       <c r="AM141" t="s" s="2">
-        <v>91</v>
+        <v>40</v>
       </c>
     </row>
     <row r="142" hidden="true">
       <c r="A142" t="s" s="2">
-        <v>513</v>
+        <v>529</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" t="s" s="2">
@@ -17425,10 +17552,10 @@
       </c>
       <c r="D142" s="2"/>
       <c r="E142" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F142" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G142" t="s" s="2">
         <v>40</v>
@@ -17440,15 +17567,17 @@
         <v>40</v>
       </c>
       <c r="J142" t="s" s="2">
-        <v>200</v>
+        <v>343</v>
       </c>
       <c r="K142" t="s" s="2">
-        <v>514</v>
+        <v>530</v>
       </c>
       <c r="L142" t="s" s="2">
-        <v>515</v>
-      </c>
-      <c r="M142" s="2"/>
+        <v>531</v>
+      </c>
+      <c r="M142" t="s" s="2">
+        <v>532</v>
+      </c>
       <c r="N142" s="2"/>
       <c r="O142" t="s" s="2">
         <v>40</v>
@@ -17497,13 +17626,13 @@
         <v>40</v>
       </c>
       <c r="AE142" t="s" s="2">
-        <v>513</v>
+        <v>529</v>
       </c>
       <c r="AF142" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG142" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="AH142" t="s" s="2">
         <v>40</v>
@@ -17526,7 +17655,7 @@
     </row>
     <row r="143" hidden="true">
       <c r="A143" t="s" s="2">
-        <v>516</v>
+        <v>533</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" t="s" s="2">
@@ -17537,7 +17666,7 @@
         <v>41</v>
       </c>
       <c r="F143" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G143" t="s" s="2">
         <v>40</v>
@@ -17549,13 +17678,13 @@
         <v>40</v>
       </c>
       <c r="J143" t="s" s="2">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="K143" t="s" s="2">
-        <v>517</v>
+        <v>253</v>
       </c>
       <c r="L143" t="s" s="2">
-        <v>518</v>
+        <v>254</v>
       </c>
       <c r="M143" s="2"/>
       <c r="N143" s="2"/>
@@ -17582,13 +17711,13 @@
         <v>40</v>
       </c>
       <c r="W143" t="s" s="2">
-        <v>162</v>
+        <v>40</v>
       </c>
       <c r="X143" t="s" s="2">
-        <v>519</v>
+        <v>40</v>
       </c>
       <c r="Y143" t="s" s="2">
-        <v>520</v>
+        <v>40</v>
       </c>
       <c r="Z143" t="s" s="2">
         <v>40</v>
@@ -17606,19 +17735,19 @@
         <v>40</v>
       </c>
       <c r="AE143" t="s" s="2">
-        <v>516</v>
+        <v>255</v>
       </c>
       <c r="AF143" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG143" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="AH143" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI143" t="s" s="2">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="AJ143" t="s" s="2">
         <v>40</v>
@@ -17630,23 +17759,23 @@
         <v>40</v>
       </c>
       <c r="AM143" t="s" s="2">
-        <v>40</v>
+        <v>256</v>
       </c>
     </row>
     <row r="144" hidden="true">
       <c r="A144" t="s" s="2">
-        <v>521</v>
+        <v>534</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" t="s" s="2">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="D144" s="2"/>
       <c r="E144" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F144" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G144" t="s" s="2">
         <v>40</v>
@@ -17658,15 +17787,17 @@
         <v>40</v>
       </c>
       <c r="J144" t="s" s="2">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="K144" t="s" s="2">
-        <v>522</v>
+        <v>95</v>
       </c>
       <c r="L144" t="s" s="2">
-        <v>523</v>
-      </c>
-      <c r="M144" s="2"/>
+        <v>258</v>
+      </c>
+      <c r="M144" t="s" s="2">
+        <v>97</v>
+      </c>
       <c r="N144" s="2"/>
       <c r="O144" t="s" s="2">
         <v>40</v>
@@ -17715,19 +17846,19 @@
         <v>40</v>
       </c>
       <c r="AE144" t="s" s="2">
-        <v>521</v>
+        <v>262</v>
       </c>
       <c r="AF144" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG144" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="AH144" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI144" t="s" s="2">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="AJ144" t="s" s="2">
         <v>40</v>
@@ -17739,44 +17870,48 @@
         <v>40</v>
       </c>
       <c r="AM144" t="s" s="2">
-        <v>40</v>
+        <v>256</v>
       </c>
     </row>
     <row r="145" hidden="true">
       <c r="A145" t="s" s="2">
-        <v>524</v>
+        <v>535</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" t="s" s="2">
-        <v>40</v>
+        <v>399</v>
       </c>
       <c r="D145" s="2"/>
       <c r="E145" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F145" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G145" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H145" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="I145" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J145" t="s" s="2">
-        <v>487</v>
+        <v>94</v>
       </c>
       <c r="K145" t="s" s="2">
-        <v>525</v>
+        <v>400</v>
       </c>
       <c r="L145" t="s" s="2">
-        <v>526</v>
-      </c>
-      <c r="M145" s="2"/>
-      <c r="N145" s="2"/>
+        <v>401</v>
+      </c>
+      <c r="M145" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="N145" t="s" s="2">
+        <v>103</v>
+      </c>
       <c r="O145" t="s" s="2">
         <v>40</v>
       </c>
@@ -17824,35 +17959,1242 @@
         <v>40</v>
       </c>
       <c r="AE145" t="s" s="2">
-        <v>524</v>
+        <v>402</v>
       </c>
       <c r="AF145" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="AG145" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="AH145" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI145" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AJ145" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK145" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL145" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM145" t="s" s="2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="146" hidden="true">
+      <c r="A146" t="s" s="2">
+        <v>536</v>
+      </c>
+      <c r="B146" s="2"/>
+      <c r="C146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D146" s="2"/>
+      <c r="E146" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F146" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J146" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="K146" t="s" s="2">
+        <v>537</v>
+      </c>
+      <c r="L146" t="s" s="2">
+        <v>538</v>
+      </c>
+      <c r="M146" s="2"/>
+      <c r="N146" s="2"/>
+      <c r="O146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P146" s="2"/>
+      <c r="Q146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE146" t="s" s="2">
+        <v>536</v>
+      </c>
+      <c r="AF146" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG146" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI146" t="s" s="2">
         <v>60</v>
       </c>
-      <c r="AJ145" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK145" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL145" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM145" t="s" s="2">
+      <c r="AJ146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL146" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM146" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="147" hidden="true">
+      <c r="A147" t="s" s="2">
+        <v>539</v>
+      </c>
+      <c r="B147" s="2"/>
+      <c r="C147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D147" s="2"/>
+      <c r="E147" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="F147" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J147" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="K147" t="s" s="2">
+        <v>540</v>
+      </c>
+      <c r="L147" t="s" s="2">
+        <v>541</v>
+      </c>
+      <c r="M147" s="2"/>
+      <c r="N147" s="2"/>
+      <c r="O147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P147" s="2"/>
+      <c r="Q147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE147" t="s" s="2">
+        <v>539</v>
+      </c>
+      <c r="AF147" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG147" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI147" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL147" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM147" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="148" hidden="true">
+      <c r="A148" t="s" s="2">
+        <v>542</v>
+      </c>
+      <c r="B148" s="2"/>
+      <c r="C148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D148" s="2"/>
+      <c r="E148" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="F148" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J148" t="s" s="2">
+        <v>526</v>
+      </c>
+      <c r="K148" t="s" s="2">
+        <v>543</v>
+      </c>
+      <c r="L148" t="s" s="2">
+        <v>544</v>
+      </c>
+      <c r="M148" s="2"/>
+      <c r="N148" s="2"/>
+      <c r="O148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P148" s="2"/>
+      <c r="Q148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE148" t="s" s="2">
+        <v>542</v>
+      </c>
+      <c r="AF148" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AG148" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI148" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL148" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM148" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="149" hidden="true">
+      <c r="A149" t="s" s="2">
+        <v>545</v>
+      </c>
+      <c r="B149" s="2"/>
+      <c r="C149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D149" s="2"/>
+      <c r="E149" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F149" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J149" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="K149" t="s" s="2">
+        <v>546</v>
+      </c>
+      <c r="L149" t="s" s="2">
+        <v>547</v>
+      </c>
+      <c r="M149" t="s" s="2">
+        <v>548</v>
+      </c>
+      <c r="N149" s="2"/>
+      <c r="O149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P149" s="2"/>
+      <c r="Q149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE149" t="s" s="2">
+        <v>545</v>
+      </c>
+      <c r="AF149" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG149" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI149" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL149" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM149" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="150" hidden="true">
+      <c r="A150" t="s" s="2">
+        <v>549</v>
+      </c>
+      <c r="B150" s="2"/>
+      <c r="C150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D150" s="2"/>
+      <c r="E150" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F150" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J150" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="K150" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="L150" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="M150" s="2"/>
+      <c r="N150" s="2"/>
+      <c r="O150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P150" s="2"/>
+      <c r="Q150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE150" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="AF150" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG150" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL150" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM150" t="s" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="151" hidden="true">
+      <c r="A151" t="s" s="2">
+        <v>550</v>
+      </c>
+      <c r="B151" s="2"/>
+      <c r="C151" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="D151" s="2"/>
+      <c r="E151" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F151" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J151" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="K151" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="L151" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="M151" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="N151" s="2"/>
+      <c r="O151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P151" s="2"/>
+      <c r="Q151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE151" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="AF151" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG151" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI151" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AJ151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL151" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM151" t="s" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="152" hidden="true">
+      <c r="A152" t="s" s="2">
+        <v>551</v>
+      </c>
+      <c r="B152" s="2"/>
+      <c r="C152" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="D152" s="2"/>
+      <c r="E152" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F152" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H152" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="I152" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J152" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="K152" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="L152" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="M152" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="N152" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="O152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P152" s="2"/>
+      <c r="Q152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE152" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="AF152" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG152" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI152" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AJ152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL152" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM152" t="s" s="2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="153" hidden="true">
+      <c r="A153" t="s" s="2">
+        <v>552</v>
+      </c>
+      <c r="B153" s="2"/>
+      <c r="C153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D153" s="2"/>
+      <c r="E153" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F153" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J153" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="K153" t="s" s="2">
+        <v>553</v>
+      </c>
+      <c r="L153" t="s" s="2">
+        <v>554</v>
+      </c>
+      <c r="M153" s="2"/>
+      <c r="N153" s="2"/>
+      <c r="O153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P153" s="2"/>
+      <c r="Q153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE153" t="s" s="2">
+        <v>552</v>
+      </c>
+      <c r="AF153" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG153" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI153" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL153" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM153" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="154" hidden="true">
+      <c r="A154" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="B154" s="2"/>
+      <c r="C154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D154" s="2"/>
+      <c r="E154" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F154" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J154" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="K154" t="s" s="2">
+        <v>556</v>
+      </c>
+      <c r="L154" t="s" s="2">
+        <v>557</v>
+      </c>
+      <c r="M154" s="2"/>
+      <c r="N154" s="2"/>
+      <c r="O154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P154" s="2"/>
+      <c r="Q154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W154" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="X154" t="s" s="2">
+        <v>558</v>
+      </c>
+      <c r="Y154" t="s" s="2">
+        <v>559</v>
+      </c>
+      <c r="Z154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE154" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="AF154" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG154" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI154" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL154" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM154" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="155" hidden="true">
+      <c r="A155" t="s" s="2">
+        <v>560</v>
+      </c>
+      <c r="B155" s="2"/>
+      <c r="C155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D155" s="2"/>
+      <c r="E155" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F155" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J155" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="K155" t="s" s="2">
+        <v>561</v>
+      </c>
+      <c r="L155" t="s" s="2">
+        <v>562</v>
+      </c>
+      <c r="M155" s="2"/>
+      <c r="N155" s="2"/>
+      <c r="O155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P155" s="2"/>
+      <c r="Q155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE155" t="s" s="2">
+        <v>560</v>
+      </c>
+      <c r="AF155" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG155" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI155" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL155" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM155" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="156" hidden="true">
+      <c r="A156" t="s" s="2">
+        <v>563</v>
+      </c>
+      <c r="B156" s="2"/>
+      <c r="C156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D156" s="2"/>
+      <c r="E156" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="F156" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J156" t="s" s="2">
+        <v>526</v>
+      </c>
+      <c r="K156" t="s" s="2">
+        <v>564</v>
+      </c>
+      <c r="L156" t="s" s="2">
+        <v>565</v>
+      </c>
+      <c r="M156" s="2"/>
+      <c r="N156" s="2"/>
+      <c r="O156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P156" s="2"/>
+      <c r="Q156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE156" t="s" s="2">
+        <v>563</v>
+      </c>
+      <c r="AF156" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AG156" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI156" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL156" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM156" t="s" s="2">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM145">
+  <autoFilter ref="A1:AM156">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -17862,7 +19204,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI144">
+  <conditionalFormatting sqref="A2:AI155">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>